<commit_message>
Updated after first e-mail
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="60">
   <si>
     <t>UUID</t>
   </si>
@@ -65,12 +65,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>The system shall store up to 1000 users</t>
-  </si>
-  <si>
-    <t>If a user tries to join and there are already 1000 users, then the system shall display "User limit reached. Try again later."</t>
-  </si>
-  <si>
     <t>NF</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>If the data fails checksum, the system shall delete the message from the message history</t>
   </si>
   <si>
-    <t xml:space="preserve">The system shall use Boost </t>
-  </si>
-  <si>
     <t>All data shall have the time of the message included</t>
   </si>
   <si>
@@ -186,6 +177,33 @@
   </si>
   <si>
     <t>If the data fails checksum, the system shall respond to the client sending the message that "Your message was not delivered"</t>
+  </si>
+  <si>
+    <t>The system shall store up to 50 users</t>
+  </si>
+  <si>
+    <t>If a user tries to join and there are already 50 users, then the system shall display "User limit reached. Try again later."</t>
+  </si>
+  <si>
+    <t>If the client requests a nick name that has already been registered, then the system shall display "Nick already in use, please enter another"</t>
+  </si>
+  <si>
+    <t>If no rooms are available then the system shall display "No rooms created, press the plus sign to create a room"</t>
+  </si>
+  <si>
+    <t>If there is no room with the given name, then they system shall display "No such room exists"</t>
+  </si>
+  <si>
+    <t>The system shall open a pop-up window when the client clicks on the plus button</t>
+  </si>
+  <si>
+    <t>The system shall create a room when the client enters the room name and clicks the submit button</t>
+  </si>
+  <si>
+    <t>If the client enters an empty string or a name that is already being used, the sytem shall display "Enter a proper name that is not being used"</t>
+  </si>
+  <si>
+    <t>The system shall use the Boost library</t>
   </si>
 </sst>
 </file>
@@ -554,16 +572,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="8.9375" style="1"/>
-    <col min="2" max="2" width="114.76171875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="141.46875" style="1" customWidth="1"/>
     <col min="3" max="16384" width="8.9375" style="1"/>
   </cols>
   <sheetData>
@@ -602,10 +620,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
-        <v>103</v>
+        <v>102.1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -613,10 +631,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>12</v>
@@ -624,10 +642,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
-        <v>105</v>
+        <v>103.1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -635,10 +653,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
-        <v>105.1</v>
+        <v>120</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>12</v>
@@ -646,10 +664,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
-        <v>105.2</v>
+        <v>120.1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -657,10 +675,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" s="1">
-        <v>106</v>
+        <v>120.2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
@@ -668,10 +686,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" s="1">
-        <v>106.1</v>
+        <v>104</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>12</v>
@@ -679,32 +697,32 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" s="1">
-        <v>107</v>
+        <v>104.1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
-        <v>107.1</v>
+        <v>105</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A13" s="1">
-        <v>108</v>
+        <v>105.1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
@@ -712,10 +730,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A14" s="1">
-        <v>108.1</v>
+        <v>105.2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -723,175 +741,175 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A15" s="1">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A16" s="1">
-        <v>110</v>
+        <v>106.1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17" s="1">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A18" s="1">
-        <v>112</v>
+        <v>107.1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A19" s="1">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A20" s="1">
-        <v>114</v>
+        <v>108.1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A21" s="1">
-        <v>114.1</v>
+        <v>109</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A22" s="1">
-        <v>114.2</v>
+        <v>110</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A23" s="1">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A24" s="1">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A25" s="1">
-        <v>116.1</v>
+        <v>113</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A26" s="1">
-        <v>116.2</v>
+        <v>114</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A27" s="1">
-        <v>117</v>
+        <v>114.1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A28" s="1">
-        <v>117.1</v>
+        <v>114.2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A29" s="1">
-        <v>117.2</v>
+        <v>115</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A30" s="1">
-        <v>117.3</v>
+        <v>116</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>12</v>
@@ -899,10 +917,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A31" s="1">
-        <v>117.4</v>
+        <v>116.1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>12</v>
@@ -910,21 +928,21 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A32" s="1">
-        <v>117.5</v>
+        <v>116.2</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A33" s="1">
-        <v>117.6</v>
+        <v>117</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>12</v>
@@ -932,10 +950,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A34" s="1">
-        <v>117.7</v>
+        <v>117.1</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>12</v>
@@ -943,10 +961,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A35" s="1">
-        <v>118</v>
+        <v>117.2</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>12</v>
@@ -954,10 +972,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A36" s="1">
-        <v>118.1</v>
+        <v>117.3</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>12</v>
@@ -965,10 +983,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A37" s="1">
-        <v>118.2</v>
+        <v>117.4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>12</v>
@@ -976,65 +994,65 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A38" s="1">
-        <v>118.3</v>
+        <v>117.5</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A39" s="1" t="s">
-        <v>40</v>
+      <c r="A39" s="1">
+        <v>117.6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A40" s="1" t="s">
-        <v>42</v>
+      <c r="A40" s="1">
+        <v>117.7</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A41" s="1" t="s">
-        <v>44</v>
+      <c r="A41" s="1">
+        <v>118</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A42" s="1" t="s">
-        <v>47</v>
+      <c r="A42" s="1">
+        <v>118.1</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A43" s="1" t="s">
-        <v>48</v>
+      <c r="A43" s="1">
+        <v>118.2</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>12</v>
@@ -1042,23 +1060,89 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A44" s="1">
+        <v>118.3</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A47" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A49" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A50" s="1">
         <v>119</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A45" s="1">
+      <c r="B50" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A51" s="1">
         <v>119.1</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="B51" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>